<commit_message>
Make processes sequences working more correct.
</commit_message>
<xml_diff>
--- a/Work items/Process mutual sequences.xlsx
+++ b/Work items/Process mutual sequences.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei_Bychko\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei_Bychko\Mine\AI\Work items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0804887D-8B5C-4B00-85C3-9716D9721FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5ACDD9-21AC-45E6-B01A-A53B672B1868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DD2F2FCB-124F-461F-86D2-FA0A83D4081E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="35">
   <si>
     <t>StartsAfterOtherStarted,</t>
   </si>
@@ -124,6 +124,21 @@
   </si>
   <si>
     <t>FBS</t>
+  </si>
+  <si>
+    <t>SBS &gt; SBF</t>
+  </si>
+  <si>
+    <t>FAF &gt; FAS</t>
+  </si>
+  <si>
+    <t>Auto-consequences:</t>
+  </si>
+  <si>
+    <t>SAF &gt; FAF, FAS, SAS</t>
+  </si>
+  <si>
+    <t>FBS &gt; SBS, SBF, FBF</t>
   </si>
 </sst>
 </file>
@@ -139,12 +154,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -159,12 +180,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A3D462-8CAB-4579-954E-46A7AD5716B2}">
-  <dimension ref="B3:Q18"/>
+  <dimension ref="B3:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N12" sqref="C7:N12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B21:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,6 +591,9 @@
       <c r="E5" t="s">
         <v>20</v>
       </c>
+      <c r="H5" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="I5" s="2" t="s">
         <v>24</v>
       </c>
@@ -587,6 +612,9 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="I6" s="2"/>
@@ -637,7 +665,9 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="H8" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="I8" s="2" t="s">
         <v>21</v>
       </c>
@@ -664,7 +694,9 @@
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
         <v>23</v>
@@ -690,7 +722,9 @@
         <v>18</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="I10" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
@@ -717,7 +751,9 @@
       <c r="H11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="2"/>
+      <c r="I11" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2" t="s">
@@ -766,6 +802,9 @@
         <v>27</v>
       </c>
       <c r="H13" s="2"/>
+      <c r="I13" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="L13" t="s">
         <v>21</v>
       </c>
@@ -786,6 +825,9 @@
       <c r="H14" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="I14" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="L14" t="s">
         <v>21</v>
       </c>
@@ -836,6 +878,31 @@
       </c>
       <c r="Q18" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B20" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B21" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B22" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B23" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B24" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>